<commit_message>
finished the predictions max r2 0.59
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/783037e7e17d67e5/NTNU/3. år/ai/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="223" documentId="8_{D74C9236-CE3D-4988-9975-6CA48F3E9495}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F5858234-C0E2-4AF2-8778-711AA6F4F341}"/>
+  <xr:revisionPtr revIDLastSave="337" documentId="8_{D74C9236-CE3D-4988-9975-6CA48F3E9495}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{301578F3-1590-4B39-8AB5-7063C46CB985}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F623F955-2D65-4B19-8F97-472A9E9C9497}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="39">
   <si>
     <t>Method</t>
   </si>
@@ -124,6 +124,33 @@
   </si>
   <si>
     <t>Random Forrest Regressor MaxDepth=4</t>
+  </si>
+  <si>
+    <t>KNN regressor n=1.</t>
+  </si>
+  <si>
+    <t>r^2 total: 0.4258551814249235</t>
+  </si>
+  <si>
+    <t>Polynomial regression, deg 2</t>
+  </si>
+  <si>
+    <t>ensemble. Randforr (32) SVR 1000 1e-3</t>
+  </si>
+  <si>
+    <t>AI, dense 512, dense 1, 4 epochs</t>
+  </si>
+  <si>
+    <t>dense 512, dense 512, dense 1, 5 epochs</t>
+  </si>
+  <si>
+    <t>sigmoid</t>
+  </si>
+  <si>
+    <t>Return the mean accuracy on the given test data and labels.</t>
+  </si>
+  <si>
+    <t>ExtratreeRegressor maxdepth=20, est=40</t>
   </si>
 </sst>
 </file>
@@ -155,7 +182,7 @@
       <name val="Var(--vscode-editor-font-family"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +192,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -181,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -195,6 +228,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C49CEF-204F-41F1-B9F7-9D7BA8FDB162}">
-  <dimension ref="A2:L37"/>
+  <dimension ref="A2:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="88" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="88" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -733,6 +768,9 @@
       <c r="K9">
         <v>0.3</v>
       </c>
+      <c r="L9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="1:12">
       <c r="D10" t="s">
@@ -1360,7 +1398,7 @@
         <v>0.39852546004075001</v>
       </c>
     </row>
-    <row r="33" spans="3:10">
+    <row r="33" spans="2:10">
       <c r="C33" t="s">
         <v>29</v>
       </c>
@@ -1386,7 +1424,7 @@
         <v>0.34921241512333101</v>
       </c>
     </row>
-    <row r="34" spans="3:10">
+    <row r="34" spans="2:10">
       <c r="C34">
         <v>4</v>
       </c>
@@ -1412,7 +1450,7 @@
         <v>0.34398083643025201</v>
       </c>
     </row>
-    <row r="35" spans="3:10">
+    <row r="35" spans="2:10">
       <c r="C35">
         <v>8</v>
       </c>
@@ -1438,7 +1476,7 @@
         <v>0.482450638607479</v>
       </c>
     </row>
-    <row r="36" spans="3:10">
+    <row r="36" spans="2:10">
       <c r="C36">
         <v>16</v>
       </c>
@@ -1464,34 +1502,392 @@
         <v>0.57169230588248598</v>
       </c>
     </row>
-    <row r="37" spans="3:10">
-      <c r="C37">
+    <row r="37" spans="2:10">
+      <c r="C37" s="5">
         <v>32</v>
       </c>
-      <c r="D37" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" t="s">
-        <v>9</v>
-      </c>
-      <c r="H37" t="s">
-        <v>10</v>
-      </c>
-      <c r="I37" t="s">
-        <v>9</v>
-      </c>
-      <c r="J37">
+      <c r="D37" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J37" s="5">
         <v>0.59234710820256997</v>
       </c>
     </row>
+    <row r="38" spans="2:10">
+      <c r="C38" s="7">
+        <v>40</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J38" s="7">
+        <v>0.59190903677141304</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" t="s">
+        <v>10</v>
+      </c>
+      <c r="I39" t="s">
+        <v>9</v>
+      </c>
+      <c r="J39">
+        <v>3.4174000000000003E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40" t="s">
+        <v>10</v>
+      </c>
+      <c r="I40" t="s">
+        <v>9</v>
+      </c>
+      <c r="J40">
+        <v>0.27392100000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" t="s">
+        <v>9</v>
+      </c>
+      <c r="J41">
+        <v>0.30882599999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H42" t="s">
+        <v>10</v>
+      </c>
+      <c r="I42" t="s">
+        <v>9</v>
+      </c>
+      <c r="J42">
+        <v>0.32458799999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10">
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" t="s">
+        <v>9</v>
+      </c>
+      <c r="J43">
+        <v>0.33065099999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10">
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" t="s">
+        <v>10</v>
+      </c>
+      <c r="I44" t="s">
+        <v>9</v>
+      </c>
+      <c r="J44">
+        <v>0.334287</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="C45">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" t="s">
+        <v>9</v>
+      </c>
+      <c r="H45" t="s">
+        <v>10</v>
+      </c>
+      <c r="I45" t="s">
+        <v>9</v>
+      </c>
+      <c r="J45">
+        <v>0.331563</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="C46">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46" t="s">
+        <v>10</v>
+      </c>
+      <c r="I46" t="s">
+        <v>9</v>
+      </c>
+      <c r="J46">
+        <v>0.34065499999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10">
+      <c r="C47">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" t="s">
+        <v>9</v>
+      </c>
+      <c r="J47">
+        <v>0.34012300000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10">
+      <c r="C48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s">
+        <v>18</v>
+      </c>
+      <c r="J48">
+        <v>2.5887267610162899E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10">
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="J49">
+        <v>4.0281531366176404E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10">
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="J50">
+        <v>4.6624639791321698E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10">
+      <c r="C51">
+        <v>5</v>
+      </c>
+      <c r="J51">
+        <v>5.59945467413003E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10">
+      <c r="C52">
+        <v>6</v>
+      </c>
+      <c r="J52">
+        <v>-5.4905274435128798E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10">
+      <c r="C53" s="1">
+        <v>8</v>
+      </c>
+      <c r="J53">
+        <v>-0.84922301876179696</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10">
+      <c r="C54" t="s">
+        <v>33</v>
+      </c>
+      <c r="J54" s="8">
+        <v>-6.0915468092361104E+28</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="B55" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55" t="s">
+        <v>34</v>
+      </c>
+      <c r="D55" t="s">
+        <v>18</v>
+      </c>
+      <c r="J55">
+        <v>-2.1816499340586701E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="B56" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" t="s">
+        <v>17</v>
+      </c>
+      <c r="J56">
+        <v>-2.1816499340586701E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10">
+      <c r="C57" t="s">
+        <v>38</v>
+      </c>
+      <c r="J57">
+        <v>0.57984439099906904</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="J20:J23 J1:J2 J4:J12 J14:J18 J25:J34 J36:J1048576">
+  <conditionalFormatting sqref="J20:J23 J1:J2 J4:J12 J14:J18 J25:J34 J36:J51 J53 J55:J1048576">
     <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="min"/>
@@ -1519,7 +1915,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J2 J4:J12 J14:J23 J25:J34 J36:J1048576">
+  <conditionalFormatting sqref="J1:J2 J4:J12 J14:J23 J25:J34 J36:J51 J53 J55:J1048576">
     <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
@@ -1561,7 +1957,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J2 J4:J12 J14:J34 J36:J1048576">
+  <conditionalFormatting sqref="J1:J2 J4:J12 J14:J34 J36:J51 J53 J55:J1048576">
     <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="min"/>
@@ -1575,7 +1971,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J12 J14:J34 J36:J1048576">
+  <conditionalFormatting sqref="J1:J12 J14:J34 J36:J51 J53 J55:J1048576">
     <cfRule type="dataBar" priority="27">
       <dataBar>
         <cfvo type="min"/>
@@ -1589,7 +1985,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J34 J36:J1048576">
+  <conditionalFormatting sqref="J1:J34 J36:J51 J53 J55:J1048576">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
@@ -1617,7 +2013,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="J1:J51 J53 J55:J1048576">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -1645,7 +2041,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J20:J23 J1:J2 J4:J12 J14:J18 J25:J34 J36:J1048576</xm:sqref>
+          <xm:sqref>J20:J23 J1:J2 J4:J12 J14:J18 J25:J34 J36:J51 J53 J55:J1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{E59F1605-3AD5-488A-8367-B59A063D6B33}">
@@ -1667,7 +2063,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J1:J2 J4:J12 J14:J23 J25:J34 J36:J1048576</xm:sqref>
+          <xm:sqref>J1:J2 J4:J12 J14:J23 J25:J34 J36:J51 J53 J55:J1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{5DEA47C6-B8FD-4134-BF77-16E535886DA5}">
@@ -1700,7 +2096,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J1:J2 J4:J12 J14:J34 J36:J1048576</xm:sqref>
+          <xm:sqref>J1:J2 J4:J12 J14:J34 J36:J51 J53 J55:J1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{126E423A-FEDB-473C-AA94-A74501802407}">
@@ -1711,7 +2107,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J1:J12 J14:J34 J36:J1048576</xm:sqref>
+          <xm:sqref>J1:J12 J14:J34 J36:J51 J53 J55:J1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4F7E9FCA-15D9-4393-A707-31E7C08EBDB2}">
@@ -1722,7 +2118,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J1:J34 J36:J1048576</xm:sqref>
+          <xm:sqref>J1:J34 J36:J51 J53 J55:J1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{55F584A5-F8E7-4655-8845-1F7D02A919B6}">
@@ -1744,7 +2140,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J1:J1048576</xm:sqref>
+          <xm:sqref>J1:J51 J53 J55:J1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>